<commit_message>
Finalizado módulo de consulta
</commit_message>
<xml_diff>
--- a/DataBase/Annotation.xlsx
+++ b/DataBase/Annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InovaFiscaliza\SCH\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715383D3-0A7A-427C-AFF6-09CA94814AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AA37E6-21F8-4622-B6BC-FBFE68A84040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="2400" windowWidth="24780" windowHeight="11715"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="154" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="183" uniqueCount="107">
   <si>
     <t>Homologação</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Data/Hora</t>
   </si>
   <si>
-    <t>00455-02-00083</t>
-  </si>
-  <si>
     <t>Atributo</t>
   </si>
   <si>
@@ -62,145 +59,304 @@
     <t>anatel_master</t>
   </si>
   <si>
+    <t>Computador</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>90eecc80-78a0-42b4-b31b-8027c4c10b1d</t>
+  </si>
+  <si>
+    <t>07/05/2024 00:48:56</t>
+  </si>
+  <si>
+    <t>01465-10-01993</t>
+  </si>
+  <si>
+    <t>WordCloud</t>
+  </si>
+  <si>
+    <t>iPhone: 18, Apple: 10, A1332: 7, Past: 5, Specifications: 4, Phones: 3, Smartphones: 3, Support: 3, price: 3, specs: 3, Cell: 2, EveryMac.com: 2, GB: 2, GSM: 2, News: 2, Sale: 2, Shopping: 2, Technical: 2, Unlocked: 2, date: 2, eBay: 2, en-us: 2, hour: 2, release: 2, support.apple.com: 2</t>
+  </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>3d94d890-e5c5-4915-a324-48a056401b9c</t>
+  </si>
+  <si>
+    <t>4c4a30ba-5563-4205-b567-8c0af80952b7</t>
+  </si>
+  <si>
+    <t>4bb1fec1-cd70-4ae2-969f-19246bbf6bef</t>
+  </si>
+  <si>
+    <t>ffb32a7c-53b8-4762-a013-0e803e2a1f94</t>
+  </si>
+  <si>
+    <t>2972df1e-bd4c-46ea-a02a-3e6cc655efbe</t>
+  </si>
+  <si>
+    <t>b222bdfc-29fa-4b1d-a106-df52f98479ea</t>
+  </si>
+  <si>
+    <t>3b1c1302-c980-40b3-8a97-c3a60d23e707</t>
+  </si>
+  <si>
+    <t>37ea5eff-45a0-4d7a-8dfb-cc3791b45b85</t>
+  </si>
+  <si>
+    <t>e2cd4b27-f372-4dc0-b8f1-298ced553288</t>
+  </si>
+  <si>
+    <t>3823faff-f870-40f0-8308-8da5a1053d0f</t>
+  </si>
+  <si>
+    <t>e01fb05f-d118-48c9-b462-0b405b5a4732</t>
+  </si>
+  <si>
+    <t>d1bdf431-7ef2-4ef9-87c8-2a26ebe78d48</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:30:14</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:30:52</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:31:34</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:35:34</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:35:47</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:35:54</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:36:00</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:36:06</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:36:21</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:36:31</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:36:35</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:37:08</t>
+  </si>
+  <si>
+    <t>10206-23-04036</t>
+  </si>
+  <si>
+    <t>06249-21-13659</t>
+  </si>
+  <si>
+    <t>05686-19-01993</t>
+  </si>
+  <si>
+    <t>05684-19-01993</t>
+  </si>
+  <si>
+    <t>05685-19-01993</t>
+  </si>
+  <si>
+    <t>12996-20-01993</t>
+  </si>
+  <si>
+    <t>12997-20-01993</t>
+  </si>
+  <si>
+    <t>12998-20-01993</t>
+  </si>
+  <si>
+    <t>12999-20-01993</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
     <t>Fornecedor</t>
   </si>
   <si>
+    <t>Outras informações</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
     <t>Casas Bahia</t>
   </si>
   <si>
-    <t>Computador</t>
-  </si>
-  <si>
-    <t>56571bc5-5469-4b61-8f37-9df5bd72a4b2</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>10/10/2023 08:55:12</t>
-  </si>
-  <si>
-    <t>49bd7b57-ab65-44a8-9371-75faf7284ce3</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:33:05</t>
-  </si>
-  <si>
-    <t>00000-00-00000</t>
-  </si>
-  <si>
-    <t>Modelo</t>
-  </si>
-  <si>
-    <t>Texto livre</t>
-  </si>
-  <si>
-    <t>47b8b214-d651-4615-b801-4c4d69249b6d</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:33:08</t>
-  </si>
-  <si>
-    <t>80c1f3eb-63b1-4010-9bac-a7a439574ba5</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:33:09</t>
-  </si>
-  <si>
-    <t>b3917efa-19e6-4cb5-a664-27766a72ecf4</t>
-  </si>
-  <si>
-    <t>fa3bb495-5f35-4168-8308-107accb2ae68</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:33:10</t>
-  </si>
-  <si>
-    <t>d54f9277-3052-4df2-ba2d-6c58e5de8657</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:34:45</t>
-  </si>
-  <si>
-    <t>03c8202d-945c-4c48-a424-d7e9b29b0396</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:34:46</t>
-  </si>
-  <si>
-    <t>20547f57-bc06-4c06-8088-63c6e2c2e55b</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:34:47</t>
-  </si>
-  <si>
-    <t>d2f29865-9a2d-4d86-8751-e2e7e3cc4d0f</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:34:48</t>
-  </si>
-  <si>
-    <t>04dec140-7972-428e-9dfb-9c26cab795d1</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:34:49</t>
-  </si>
-  <si>
-    <t>df2b32a9-c4d6-4744-9f40-1aac8c35a5a1</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:34:57</t>
-  </si>
-  <si>
-    <t>6429f0bf-c175-4038-85c6-fd0c6151128f</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:35:35</t>
-  </si>
-  <si>
-    <t>37ea9ea3-acfe-4d4b-b5a0-45e510652b3b</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:43:24</t>
-  </si>
-  <si>
-    <t>d8bac1b6-56a8-44a7-8988-901c3eb7b4ee</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:54:11</t>
-  </si>
-  <si>
-    <t>b78efc7c-6c96-488b-a7db-4bb754d000f0</t>
-  </si>
-  <si>
-    <t>25/04/2024 20:55:13</t>
-  </si>
-  <si>
-    <t>3dc06c4c-d352-45bf-a775-8182ec54706c</t>
-  </si>
-  <si>
-    <t>25/04/2024 21:00:43</t>
-  </si>
-  <si>
-    <t>131fa976-7f1d-466d-8fd2-30c898363e7c</t>
-  </si>
-  <si>
-    <t>25/04/2024 21:00:51</t>
-  </si>
-  <si>
-    <t>a56853e2-2228-4a83-82ed-bcba59790691</t>
-  </si>
-  <si>
-    <t>25/04/2024 21:01:05</t>
-  </si>
-  <si>
-    <t>82b909b8-7b08-4d7b-a108-332bb40abdbf</t>
-  </si>
-  <si>
-    <t>daed8065-0dff-4bd8-99dd-7d4db123dc8f</t>
-  </si>
-  <si>
-    <t>25/04/2024 21:01:06</t>
+    <t>Qualquer coisa que faça sentido na fiscalização pra fins de busca na base</t>
+  </si>
+  <si>
+    <t>AP1901: 7, Past: 5, Access: 3, PDF: 3, Point: 3, Promotional: 3, View: 3, APOD: 2, Images: 2, January: 2, NASA: 2, News: 2, Pen: 2, Product: 2, Shopping: 2, hour: 2, 4in1: 1, AC1900: 1, AP: 1, AP-1: 1, AP-11: 1, AP-1901-Inventories: 1, AP500: 1, Adhesion: 1, Aerospace: 1</t>
+  </si>
+  <si>
+    <t>iPhone: 18, A2221: 14, Apple: 9, Past: 5, Phones: 5, model: 5, 64GB: 3, A2223: 3, Smartphones: 3, everymac.com: 3, specs: 3, A2111: 2, Cell: 2, Community: 2, Mac: 2, Number: 2, Shopping: 2, Unlocked: 2, country: 2, discussions.apple.com: 2, hour: 2, systems: 2, work: 2, 6.1-inch: 1, A2222: 1</t>
+  </si>
+  <si>
+    <t>A2215: 14, iPhone: 12, Pro: 9, Apple: 6, Past: 5, A2160: 4, A2217: 4, Model: 4, country: 3, everymac.com: 3, A2216: 2, Blog: 2, Mac: 2, Prices: 2, Specs: 2, devices: 2, discussions.apple.com: 2, hour: 2, phone: 2, 11-Upgraded-Capacity-Replacement-Professional: 1, 256GB: 1, 3600mAh: 1, A2221: 1, Ability: 1, Amazfit: 1</t>
+  </si>
+  <si>
+    <t>A2218: 14, iPhone: 14, Max: 13, Pro: 13, A2161: 5, Apple: 5, Past: 5, A2220: 4, A2219: 3, IMEI: 2, Model: 2, Price: 2, Specs: 2, country: 2, findphones-detail: 2, hour: 2, phone: 2, www.gari.info: 2, 12634-Apple-iPhone-11-Pro-Max-A2218-2: 1, 256GB: 1, 64GB: 1, Ability: 1, Amazon.com: 1, Books: 1, Central: 1</t>
+  </si>
+  <si>
+    <t>iPhone: 16, A2403: 15, Apple: 10, Past: 5, Global: 4, Model: 3, everymac.com: 3, specs: 3, 64GB: 2, A2404: 2, Black: 2, Information: 2, Mac: 2, News: 2, Sim: 2, hour: 2, tmobile: 2, 128GB: 1, 256GB: 1, 5G: 1, A2172: 1, A2402: 1, Blue: 1, Books: 1, Condition: 1</t>
+  </si>
+  <si>
+    <t>iPhone: 26, mini: 22, Apple: 9, Past: 5, Reddit: 4, 64GB: 3, Specifications: 3, Unlocked: 3, iPhone12Mini: 3, phone: 3, review: 3, 128GB: 2, Black: 2, News: 2, Refurbished: 2, Renewed: 2, Shopping: 2, Technical: 2, hour: 2, r: 2, released: 2, size: 2, still: 2, worth: 2, www.amazon.com: 2</t>
+  </si>
+  <si>
+    <t>iPhone: 29, Pro: 20, Apple: 9, Past: 5, 128GB: 4, Blue: 4, Refurbished: 4, Unlocked: 4, shop: 4, www.apple.com: 4, Pacific: 3, Prices: 3, iphone-12-pro: 3, Directory: 2, Max: 2, News: 2, Walmart: 2, buying: 2, compare: 2, hour: 2, phone: 2, product: 2, 18.05/mo: 1, 256GB: 1, 5G: 1</t>
+  </si>
+  <si>
+    <t>iPhone: 31, Pro: 23, Max: 22, Apple: 11, 128GB: 6, Unlocked: 6, Past: 5, Blue: 4, vs: 4, Compare: 3, Pacific: 3, Shopping: 3, price: 3, www.apple.com: 3, 256GB: 2, 5G: 2, Apple-iPhone-128GB-Pacific-Blue: 2, Graphite: 2, Refurbished: 2, Review: 2, Specifications: 2, Verizon: 2, Walmart: 2, hour: 2, www.amazon.com: 2</t>
+  </si>
+  <si>
+    <t>IPHONE 11</t>
+  </si>
+  <si>
+    <t>7123fb2f-5c74-4c1c-bcb1-2bba97ec3c4a</t>
+  </si>
+  <si>
+    <t>bb0fffa8-4717-4205-a52f-b56b5d474135</t>
+  </si>
+  <si>
+    <t>08/05/2024 09:46:28</t>
+  </si>
+  <si>
+    <t>08/05/2024 10:01:01</t>
+  </si>
+  <si>
+    <t>01731-23-15463</t>
+  </si>
+  <si>
+    <t>EAN</t>
+  </si>
+  <si>
+    <t>01010101010101010</t>
+  </si>
+  <si>
+    <t>Module: 7, Past: 5, 4G: 3, Chipset: 2, Embedded: 2, Images: 2, PDF: 2, Qualcomm: 2, Routing: 2, Search: 2, Videos: 2, View: 2, down_31: 2, file: 2, hour: 2, item: 2, static: 2, upload: 2, www.aliexpress.com: 2, www.szlbt.com: 2, 器: 2, 嵌入式: 2, 模组: 2, 由: 2, 路: 2</t>
+  </si>
+  <si>
+    <t>4d070f42-976e-4ea2-ba0d-48b9c70e3381</t>
+  </si>
+  <si>
+    <t>cd0ba100-a500-4205-a3a0-bbab5e8f8686</t>
+  </si>
+  <si>
+    <t>063d4365-0003-4e87-b953-7579f6291c5b</t>
+  </si>
+  <si>
+    <t>8bae06ac-cd91-4513-98ce-14005af55379</t>
+  </si>
+  <si>
+    <t>2bb04b43-ce05-4967-9d63-791d0f514198</t>
+  </si>
+  <si>
+    <t>10/05/2024 10:24:29</t>
+  </si>
+  <si>
+    <t>10/05/2024 10:29:59</t>
+  </si>
+  <si>
+    <t>10/05/2024 10:34:34</t>
+  </si>
+  <si>
+    <t>10/05/2024 10:35:03</t>
+  </si>
+  <si>
+    <t>10/05/2024 10:35:16</t>
+  </si>
+  <si>
+    <t>16759-20-00953</t>
+  </si>
+  <si>
+    <t>00171-03-01801</t>
+  </si>
+  <si>
+    <t>Samsung: 16, DS: 12, SM-G996B: 12, S21: 11, 5G: 9, Galaxy: 9, Plus: 9, Phones: 8, 256GB: 5, Past: 5, Unlocked: 3, 8GB: 2, Cell: 2, Celulares: 2, Desbloqueados: 2, Home: 2, Review: 2, Walmart: 2, g996b: 2, hour: 2, price: 2, specifications: 2, www.amazon.com: 2, www.walmart.com: 2, 256+8GB: 1</t>
+  </si>
+  <si>
+    <t>EP450</t>
+  </si>
+  <si>
+    <t>PowerSafe: 19, Batteries: 16, 12VE38: 10, EnerSys: 10, V: 10, 12V: 5, Front: 5, Past: 5, Terminal: 5, 38Ah: 4, Replacement: 3, 12V38f: 2, PDF: 2, UPS: 2, hour: 2, products: 2, www.enersys.com: 2, ®: 2, 190F: 1, 2V400: 1, 35w: 1, 8Ah: 1, Acid: 1, Bleibatterien: 1, Books: 1</t>
+  </si>
+  <si>
+    <t>Poly: 24, Edge: 23, E400: 16, Phone: 14, IP: 11, Desk: 6, Past: 5, Series: 4, Shop: 3, Communication: 2, CookandBoardman.com: 2, E: 2, HP: 2, Images: 2, Shop4Tele.com: 2, View: 2, hour: 2, products: 2, www.hp.com: 2, 82M93AA: 1, 8x8: 1, Ad·www: 1, Amazon.com: 1, BUSINESS: 1, Books: 1</t>
+  </si>
+  <si>
+    <t>5ac5ceb6-4201-43a5-a104-7a4271045db9</t>
+  </si>
+  <si>
+    <t>f2542eda-1b87-4939-8529-2c0e09b03ee9</t>
+  </si>
+  <si>
+    <t>10/05/2024 12:48:31</t>
+  </si>
+  <si>
+    <t>10/05/2024 12:50:03</t>
+  </si>
+  <si>
+    <t>11243-21-01993</t>
+  </si>
+  <si>
+    <t>10986-22-01993</t>
+  </si>
+  <si>
+    <t>iPhone: 18, A2643: 16, Max: 13, Pro: 13, Apple: 8, Past: 5, model: 5, A2484: 3, A2641: 3, Global: 3, number: 3, phone: 3, 5G: 2, A2644: 2, EveryMac.com: 2, IMEI: 2, Smartphones: 2, Support: 2, hour: 2, specs: 2, 1TB: 1, 4G: 1, A2645: 1, Bands: 1, Books: 1</t>
+  </si>
+  <si>
+    <t>iPhone: 20, A2882: 15, Apple: 12, 128GB: 5, Past: 5, Smartphone: 4, model: 3, specs: 3, 5G: 2, A2884: 2, GB: 2, IMEI: 2, Midnight: 2, Nano: 2, Number: 2, Price: 2, Sim: 2, country: 2, eSIM: 2, hour: 2, www.etoren.com: 2, A2649: 1, A2881: 1, A2883: 1, Books: 1</t>
+  </si>
+  <si>
+    <t>c78a854d-f943-4600-b170-af34762a97f4</t>
+  </si>
+  <si>
+    <t>dd04205c-7ec1-4932-93cb-063644ca72c8</t>
+  </si>
+  <si>
+    <t>b61bda3a-5759-4667-8ac2-6c57ae15f38d</t>
+  </si>
+  <si>
+    <t>10/05/2024 18:17:39</t>
+  </si>
+  <si>
+    <t>10/05/2024 18:17:46</t>
+  </si>
+  <si>
+    <t>10/05/2024 18:17:50</t>
+  </si>
+  <si>
+    <t>05495-19-09931</t>
+  </si>
+  <si>
+    <t>00054-15-09523</t>
+  </si>
+  <si>
+    <t>00054-09-05099</t>
+  </si>
+  <si>
+    <t>AMX: 14, Acendo: 11, Vibe: 11, ACV-5100: 10, Conferencing: 8, KR: 5, Past: 5, Soundbar: 5, 5100BL: 4, Acv: 4, Camera: 4, Bar: 3, Sound: 3, Shopping: 2, Videos: 2, hour: 2, manual: 2, product: 2, tools: 2, www.amx.com: 2, 1440852-REG: 1, ACR-5100: 1, AMX-ACV-5100-Acendo-Vibe-Confere: 1, AMX-Acendo-Conferencing-Sound-Camera: 1, Audio: 1</t>
+  </si>
+  <si>
+    <t>DigiMod: 9, Audio: 7, Powersoft: 7, DIGIMOD-I: 6, Pro: 6, SKP: 6, Microphones: 5, Past: 5, products: 4, Digital: 3, Wireless: 3, Images: 2, Shopping: 2, View: 2, amp-modules: 2, hour: 2, tools: 2, www.powersoft.com: 2, www.skpaudio.com: 2, 3004PFC2: 1, 3004PFC4: 1, 4HV: 1, Amazon.com: 1, Amplifiers: 1, Books: 1</t>
+  </si>
+  <si>
+    <t>Epen: 17, Past: 5, ePEN2: 4, login: 3, Emory: 2, Hair: 2, Pearson: 2, Removal: 2, Set: 2, hour: 2, wiki: 2, Atlanta: 1, Books: 1, Creative: 1, Dark: 1, Dictionary: 1, E: 1, Electrolysis: 1, Employee: 1, Free: 1, GA: 1, Google: 1, Help: 1, Images: 1, Learn: 1</t>
   </si>
 </sst>
 </file>
@@ -258,12 +414,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
@@ -601,11 +763,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99FF610-CB6D-4AA1-8BD3-CFE0C117587C}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -613,18 +773,19 @@
     <col min="2" max="5" width="21.42578125" style="2" customWidth="true"/>
     <col min="6" max="6" width="28.5703125" style="2" customWidth="true"/>
     <col min="7" max="7" width="85.7109375" style="2" customWidth="true"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="10.85546875" style="4" customWidth="true"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -633,493 +794,663 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.25">
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>18</v>
+        <v>59</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>61</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>18</v>
+        <v>62</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>18</v>
+        <v>70</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>18</v>
+        <v>52</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>18</v>
+        <v>83</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>18</v>
+        <v>84</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>18</v>
+        <v>85</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>18</v>
+        <v>86</v>
+      </c>
+      <c r="H21" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>18</v>
+        <v>93</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>